<commit_message>
Lending and Retrieving Books
</commit_message>
<xml_diff>
--- a/LMS/bin/Debug/net8.0-windows/LMS.xlsx
+++ b/LMS/bin/Debug/net8.0-windows/LMS.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\SandBox\LibraryManagementSystem\LMS\LMS\bin\Debug\net8.0-windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9BF5C0-ADAE-41CF-A6B7-67B4E3D6E5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C51386-08F4-43F6-AB05-B29B8E9E68A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Members" sheetId="2" r:id="rId1"/>
     <x:sheet name="Books" sheetId="3" r:id="rId2"/>
+    <x:sheet name="Lendings" sheetId="4" r:id="rId3"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="0"/>
@@ -45,6 +46,9 @@
     <x:t>Normal</x:t>
   </x:si>
   <x:si>
+    <x:t>, 10003</x:t>
+  </x:si>
+  <x:si>
     <x:t>Masoud</x:t>
   </x:si>
   <x:si>
@@ -63,12 +67,18 @@
     <x:t>Gholami</x:t>
   </x:si>
   <x:si>
+    <x:t xml:space="preserve">, </x:t>
+  </x:si>
+  <x:si>
     <x:t>Kambiz</x:t>
   </x:si>
   <x:si>
     <x:t>Kambizi</x:t>
   </x:si>
   <x:si>
+    <x:t>, 10007</x:t>
+  </x:si>
+  <x:si>
     <x:t>Sakine</x:t>
   </x:si>
   <x:si>
@@ -81,6 +91,9 @@
     <x:t>Sharafollahi</x:t>
   </x:si>
   <x:si>
+    <x:t>, 10009</x:t>
+  </x:si>
+  <x:si>
     <x:t>Hosein</x:t>
   </x:si>
   <x:si>
@@ -93,6 +106,9 @@
     <x:t>Soosani</x:t>
   </x:si>
   <x:si>
+    <x:t>, 10010</x:t>
+  </x:si>
+  <x:si>
     <x:t>Nazanin</x:t>
   </x:si>
   <x:si>
@@ -229,6 +245,9 @@
   </x:si>
   <x:si>
     <x:t>Fun</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024/7/17</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -575,7 +594,7 @@
   <x:dimension ref="A1:F19"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="F2" sqref="F2"/>
+      <x:selection activeCell="F1" sqref="F1"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,16 +635,19 @@
       <x:c r="E2" s="0">
         <x:v>100</x:v>
       </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
     </x:row>
     <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A3" s="0">
         <x:v>1004</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>2</x:v>
@@ -639,10 +661,10 @@
         <x:v>1005</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
         <x:v>6</x:v>
@@ -656,16 +678,19 @@
         <x:v>1006</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
       <x:c r="E5" s="0">
         <x:v>100</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -673,16 +698,19 @@
         <x:v>1007</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="E6" s="0">
         <x:v>100</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -690,10 +718,10 @@
         <x:v>1008</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
         <x:v>6</x:v>
@@ -707,16 +735,19 @@
         <x:v>1009</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="E8" s="0">
         <x:v>200</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -724,10 +755,10 @@
         <x:v>1010</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
         <x:v>2</x:v>
@@ -741,16 +772,19 @@
         <x:v>1011</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
       <x:c r="E10" s="0">
         <x:v>400</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -758,10 +792,10 @@
         <x:v>1012</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
         <x:v>6</x:v>
@@ -775,10 +809,10 @@
         <x:v>1013</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
         <x:v>6</x:v>
@@ -792,10 +826,10 @@
         <x:v>1014</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
         <x:v>6</x:v>
@@ -809,10 +843,10 @@
         <x:v>1015</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
         <x:v>6</x:v>
@@ -826,10 +860,10 @@
         <x:v>1017</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
         <x:v>6</x:v>
@@ -843,10 +877,10 @@
         <x:v>1018</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
         <x:v>6</x:v>
@@ -860,10 +894,10 @@
         <x:v>1019</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
         <x:v>2</x:v>
@@ -877,10 +911,10 @@
         <x:v>1020</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
         <x:v>6</x:v>
@@ -894,10 +928,10 @@
         <x:v>1021</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
         <x:v>6</x:v>
@@ -920,10 +954,10 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E9"/>
+  <x:dimension ref="A1:E10"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
-      <x:selection activeCell="E5" sqref="E5"/>
+      <x:selection activeCell="E1" sqref="E1"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,13 +967,13 @@
         <x:v>10002</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="E1" s="0">
         <x:v>1002</x:v>
@@ -950,13 +984,16 @@
         <x:v>10003</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="E2" s="0">
+        <x:v>1003</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -964,13 +1001,13 @@
         <x:v>10004</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -978,13 +1015,13 @@
         <x:v>10005</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -992,13 +1029,13 @@
         <x:v>10006</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="E5" s="0">
         <x:v>1002</x:v>
@@ -1009,13 +1046,16 @@
         <x:v>10007</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="E6" s="0">
+        <x:v>1007</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1023,13 +1063,13 @@
         <x:v>10008</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1037,13 +1077,16 @@
         <x:v>10009</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="E8" s="0">
+        <x:v>1009</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1051,27 +1094,30 @@
         <x:v>10010</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>65</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:5">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="E9" s="0">
+        <x:v>1011</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A10" s="0">
         <x:v>100011</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1081,4 +1127,68 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{3922FDCC-510A-4366-8D8C-E53DC6242FE7}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:3">
+      <x:c r="A1" s="0">
+        <x:v>10003</x:v>
+      </x:c>
+      <x:c r="B1" s="0">
+        <x:v>1003</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3">
+      <x:c r="A2" s="0">
+        <x:v>10009</x:v>
+      </x:c>
+      <x:c r="B2" s="0">
+        <x:v>1009</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="A3" s="0">
+        <x:v>10007</x:v>
+      </x:c>
+      <x:c r="B3" s="0">
+        <x:v>1007</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
+      <x:c r="A4" s="0">
+        <x:v>10010</x:v>
+      </x:c>
+      <x:c r="B4" s="0">
+        <x:v>1011</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
Added Score, Importing and Exporting excel files.
</commit_message>
<xml_diff>
--- a/LMS/bin/Debug/net8.0-windows/LMS.xlsx
+++ b/LMS/bin/Debug/net8.0-windows/LMS.xlsx
@@ -131,6 +131,9 @@
   </x:si>
   <x:si>
     <x:t>Jesus</x:t>
+  </x:si>
+  <x:si>
+    <x:t>, 10005</x:t>
   </x:si>
   <x:si>
     <x:t>Zhale</x:t>
@@ -854,16 +857,19 @@
       <x:c r="E14" s="0">
         <x:v>100</x:v>
       </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
     </x:row>
     <x:row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A15" s="0">
         <x:v>1017</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
         <x:v>6</x:v>
@@ -877,10 +883,10 @@
         <x:v>1018</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
         <x:v>6</x:v>
@@ -894,10 +900,10 @@
         <x:v>1019</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
         <x:v>2</x:v>
@@ -911,10 +917,10 @@
         <x:v>1020</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
         <x:v>6</x:v>
@@ -928,10 +934,10 @@
         <x:v>1021</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
         <x:v>6</x:v>
@@ -967,13 +973,13 @@
         <x:v>10002</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E1" s="0">
         <x:v>1002</x:v>
@@ -984,13 +990,13 @@
         <x:v>10003</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="E2" s="0">
         <x:v>1003</x:v>
@@ -1001,13 +1007,13 @@
         <x:v>10004</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1015,13 +1021,16 @@
         <x:v>10005</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="E4" s="0">
+        <x:v>1015</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1029,13 +1038,13 @@
         <x:v>10006</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E5" s="0">
         <x:v>1002</x:v>
@@ -1046,13 +1055,13 @@
         <x:v>10007</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E6" s="0">
         <x:v>1007</x:v>
@@ -1063,13 +1072,13 @@
         <x:v>10008</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1077,13 +1086,13 @@
         <x:v>10009</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="E8" s="0">
         <x:v>1009</x:v>
@@ -1094,13 +1103,13 @@
         <x:v>10010</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="E9" s="0">
         <x:v>1011</x:v>
@@ -1111,13 +1120,13 @@
         <x:v>100011</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1148,7 +1157,7 @@
         <x:v>1003</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:3">
@@ -1159,7 +1168,7 @@
         <x:v>1009</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3">
@@ -1170,7 +1179,7 @@
         <x:v>1007</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3">
@@ -1181,7 +1190,18 @@
         <x:v>1011</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:3">
+      <x:c r="A5" s="0">
+        <x:v>10005</x:v>
+      </x:c>
+      <x:c r="B5" s="0">
+        <x:v>1015</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>